<commit_message>
análises - revisão da exportação
</commit_message>
<xml_diff>
--- a/dados/csv/2023/1/sint_qtd_por_modalidade_2023.xlsx
+++ b/dados/csv/2023/1/sint_qtd_por_modalidade_2023.xlsx
@@ -14,17 +14,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>geral_modalidade</t>
   </si>
   <si>
-    <t>geral_status</t>
-  </si>
-  <si>
     <t>total</t>
   </si>
   <si>
+    <t>total_sucesso</t>
+  </si>
+  <si>
+    <t>total_falha</t>
+  </si>
+  <si>
     <t>aon</t>
   </si>
   <si>
@@ -32,18 +35,6 @@
   </si>
   <si>
     <t>sub</t>
-  </si>
-  <si>
-    <t>failed</t>
-  </si>
-  <si>
-    <t>successful</t>
-  </si>
-  <si>
-    <t>waiting_funds</t>
-  </si>
-  <si>
-    <t>published</t>
   </si>
 </sst>
 </file>
@@ -401,13 +392,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -417,93 +408,50 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1335</v>
+      </c>
+      <c r="C2">
+        <v>830</v>
+      </c>
+      <c r="D2">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>1468</v>
+      </c>
+      <c r="C3">
+        <v>1383</v>
+      </c>
+      <c r="D3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>827</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
+      <c r="B4">
+        <v>684</v>
       </c>
       <c r="C4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>1380</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9">
-        <v>57</v>
+        <v>152</v>
+      </c>
+      <c r="D4">
+        <v>532</v>
       </c>
     </row>
   </sheetData>

</xml_diff>